<commit_message>
tail end of persName refs
</commit_message>
<xml_diff>
--- a/z-support-files/Spectral-finalize/0_lists3/tags-with-IDs.xlsx
+++ b/z-support-files/Spectral-finalize/0_lists3/tags-with-IDs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="15560" tabRatio="1000" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="8700" windowHeight="15560" tabRatio="1000" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="term-unusued" sheetId="3" r:id="rId1"/>
@@ -2615,7 +2615,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="556">
+  <cellStyleXfs count="884">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3065,6 +3065,334 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3236,7 +3564,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="556">
+  <cellStyles count="884">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3517,6 +3845,170 @@
     <cellStyle name="Followed Hyperlink" xfId="551" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="553" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="555" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="557" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="559" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="561" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="563" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="565" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="567" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="569" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="571" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="573" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="575" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="577" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="579" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="581" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="583" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="585" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="587" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="589" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="591" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="593" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="595" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="597" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="599" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="601" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="603" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="605" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="607" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="609" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="611" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="613" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="615" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="617" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="619" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="621" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="623" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="625" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="627" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="629" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="631" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="633" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="635" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="637" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="639" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="641" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="643" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="645" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="647" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="649" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="651" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="653" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="655" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="657" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="659" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="661" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="663" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="665" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="667" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="669" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="671" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="673" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="675" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="677" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="679" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="681" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="683" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="685" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="687" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="689" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="691" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="693" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="695" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="697" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="699" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="701" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="703" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="705" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="707" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="709" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="711" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="713" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="715" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="717" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="719" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="721" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="723" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="725" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="727" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="729" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="731" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="733" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="735" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="737" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="739" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="741" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="743" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="745" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="747" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="749" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="751" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="753" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="755" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="757" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="759" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="761" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="763" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="765" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="767" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="769" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="771" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="773" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="775" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="777" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="779" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="781" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="783" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="785" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="787" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="789" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="791" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="793" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="795" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="797" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="799" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="801" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="803" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="805" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="807" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="809" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="811" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="813" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="815" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="817" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="819" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="821" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="823" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="825" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="827" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="829" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="831" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="833" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="835" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="837" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="839" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="841" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="843" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="845" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="847" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="849" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="851" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="853" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="855" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="857" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="859" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="861" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="863" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="865" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="867" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="869" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="871" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="873" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="875" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="877" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="879" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="881" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="883" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3792,6 +4284,170 @@
     <cellStyle name="Hyperlink" xfId="550" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="552" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="554" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="556" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="558" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="560" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="562" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="564" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="566" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="568" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="570" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="572" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="574" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="576" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="578" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="580" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="582" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="584" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="586" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="588" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="590" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="592" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="594" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="596" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="598" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="600" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="602" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="604" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="606" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="608" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="610" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="612" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="614" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="616" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="618" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="620" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="622" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="624" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="626" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="628" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="630" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="632" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="634" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="636" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="638" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="640" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="642" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="644" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="646" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="648" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="650" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="652" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="654" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="656" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="658" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="660" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="662" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="664" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="666" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="668" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="670" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="672" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="674" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="676" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="678" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="680" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="682" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="684" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="686" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="688" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="690" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="692" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="694" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="696" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="698" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="700" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="702" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="704" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="706" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="708" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="710" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="712" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="714" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="716" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="718" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="720" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="722" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="724" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="726" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="728" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="730" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="732" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="734" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="736" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="738" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="740" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="742" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="744" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="746" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="748" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="750" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="752" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="754" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="756" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="758" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="760" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="762" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="764" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="766" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="768" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="770" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="772" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="774" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="776" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="778" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="780" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="782" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="784" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="786" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="788" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="790" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="792" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="794" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="796" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="798" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="800" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="802" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="804" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="806" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="808" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="810" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="812" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="814" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="816" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="818" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="820" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="822" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="824" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="826" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="828" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="830" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="832" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="834" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="836" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="838" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="840" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="842" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="844" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="846" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="848" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="850" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="852" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="854" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="856" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="858" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="860" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="862" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="864" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="866" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="868" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="870" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="872" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="874" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="876" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="878" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="880" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="882" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
@@ -7175,8 +7831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H132"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C57" sqref="B1:C57"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8923,6 +9579,7 @@
       <c r="B105" s="10" t="s">
         <v>160</v>
       </c>
+      <c r="C105" s="14"/>
       <c r="D105" s="21"/>
       <c r="E105" s="21"/>
       <c r="F105" s="12" t="s">
@@ -8943,6 +9600,7 @@
       <c r="B106" s="10" t="s">
         <v>166</v>
       </c>
+      <c r="C106" s="14"/>
       <c r="D106" s="21"/>
       <c r="E106" s="21"/>
       <c r="F106" s="12" t="s">
@@ -8963,6 +9621,7 @@
       <c r="B107" s="10" t="s">
         <v>158</v>
       </c>
+      <c r="C107" s="14"/>
       <c r="D107" s="21"/>
       <c r="E107" s="21"/>
       <c r="F107" s="12" t="s">
@@ -8983,6 +9642,7 @@
       <c r="B108" s="10" t="s">
         <v>165</v>
       </c>
+      <c r="C108" s="14"/>
       <c r="D108" s="21"/>
       <c r="E108" s="21"/>
       <c r="F108" s="12" t="s">
@@ -9000,6 +9660,7 @@
       <c r="B109" s="10" t="s">
         <v>136</v>
       </c>
+      <c r="C109" s="14"/>
       <c r="D109" s="21"/>
       <c r="E109" s="21"/>
     </row>
@@ -9007,6 +9668,7 @@
       <c r="B110" s="10" t="s">
         <v>152</v>
       </c>
+      <c r="C110" s="14"/>
       <c r="D110" s="21"/>
       <c r="E110" s="21"/>
     </row>
@@ -9014,6 +9676,7 @@
       <c r="B111" s="10" t="s">
         <v>164</v>
       </c>
+      <c r="C111" s="14"/>
       <c r="D111" s="21"/>
       <c r="E111" s="21"/>
     </row>
@@ -9178,9 +9841,7 @@
       <c r="E131" s="17"/>
     </row>
     <row r="132" spans="2:5">
-      <c r="B132" s="18">
-        <v>199</v>
-      </c>
+      <c r="B132" s="18"/>
     </row>
   </sheetData>
   <sortState ref="B1:F128">
@@ -9205,8 +9866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>